<commit_message>
save from student list func done.
</commit_message>
<xml_diff>
--- a/Data/ogrenci_listesi.xlsx
+++ b/Data/ogrenci_listesi.xlsx
@@ -2575,7 +2575,7 @@
     <col min="4" max="4" style="3" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -2659,7 +2659,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
       <c r="A28" s="2" t="s">
         <v>22</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
       <c r="A30" s="2" t="s">
         <v>22</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
       <c r="A31" s="2" t="s">
         <v>22</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
       <c r="A32" s="2" t="s">
         <v>24</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
       <c r="A33" s="2" t="s">
         <v>24</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
       <c r="A34" s="2" t="s">
         <v>24</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
       <c r="A35" s="2" t="s">
         <v>24</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
       <c r="A36" s="2" t="s">
         <v>24</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
       <c r="A37" s="2" t="s">
         <v>24</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
       <c r="A38" s="2" t="s">
         <v>24</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
       <c r="A39" s="2" t="s">
         <v>24</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
       <c r="A40" s="2" t="s">
         <v>24</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
       <c r="A41" s="2" t="s">
         <v>24</v>
       </c>
@@ -3149,7 +3149,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
       <c r="A42" s="2" t="s">
         <v>24</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
       <c r="A43" s="2" t="s">
         <v>24</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
       <c r="A44" s="2" t="s">
         <v>24</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
       <c r="A45" s="2" t="s">
         <v>24</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
       <c r="A46" s="2" t="s">
         <v>24</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
       <c r="A47" s="2" t="s">
         <v>26</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
       <c r="A48" s="2" t="s">
         <v>26</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
       <c r="A49" s="2" t="s">
         <v>26</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
       <c r="A50" s="2" t="s">
         <v>26</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
       <c r="A51" s="2" t="s">
         <v>26</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25">
       <c r="A52" s="2" t="s">
         <v>26</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25">
       <c r="A53" s="2" t="s">
         <v>26</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25">
       <c r="A54" s="2" t="s">
         <v>26</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25">
       <c r="A55" s="2" t="s">
         <v>26</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25">
       <c r="A56" s="2" t="s">
         <v>26</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25">
       <c r="A57" s="2" t="s">
         <v>26</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25">
       <c r="A58" s="2" t="s">
         <v>26</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25">
       <c r="A59" s="2" t="s">
         <v>26</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="17.25">
       <c r="A60" s="2" t="s">
         <v>26</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="17.25">
       <c r="A61" s="2" t="s">
         <v>26</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="17.25">
       <c r="A62" s="2" t="s">
         <v>28</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="17.25">
       <c r="A63" s="2" t="s">
         <v>28</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="17.25">
       <c r="A64" s="2" t="s">
         <v>28</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="17.25">
       <c r="A65" s="2" t="s">
         <v>28</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="17.25">
       <c r="A66" s="2" t="s">
         <v>28</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="17.25">
       <c r="A67" s="2" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Student list menu done.
</commit_message>
<xml_diff>
--- a/Data/ogrenci_listesi.xlsx
+++ b/Data/ogrenci_listesi.xlsx
@@ -3513,7 +3513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="17.25">
       <c r="A68" s="2" t="s">
         <v>28</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="17.25">
       <c r="A69" s="2" t="s">
         <v>28</v>
       </c>

</xml_diff>